<commit_message>
updated migration file with bug fix and added pre-seeded data to markets table.
</commit_message>
<xml_diff>
--- a/model/farmers_sample_data.xlsx
+++ b/model/farmers_sample_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codeop\Final Project\FS7-farmers-marketplace\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB5609-B8FA-490C-A411-0425117BEFAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F61A86-9AD7-49B7-B6E5-983A68FD2A36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{9651B94E-1C84-4B72-9806-3FDA90C5FBC5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15852" windowHeight="10464" xr2:uid="{9651B94E-1C84-4B72-9806-3FDA90C5FBC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Markets" sheetId="5" r:id="rId1"/>
@@ -845,7 +845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -865,6 +865,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D56FBBA-0145-4BFA-9717-E05A70ED09A0}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2112,7 +2113,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2358,8 +2359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4BBA68-1C47-449B-8EAF-49FA2F7DE03F}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2394,34 +2395,34 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="11" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2969,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA795AE-AAAB-4C19-8827-0AB6B8F3630D}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>